<commit_message>
ENabling all testcases with some changes
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC31_Verify_PlaceOrder_WithMultiple_Items.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC31_Verify_PlaceOrder_WithMultiple_Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00077FA7-9FBD-4812-B018-54B540C18F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B34A7AB-43EF-43BF-B839-64FD4EE2DB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -715,7 +715,7 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,8 +1483,8 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
-      <c r="B61" s="11" t="s">
-        <v>29</v>
+      <c r="B61" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="11"/>

</xml_diff>